<commit_message>
Add TDD By Liuziqian
</commit_message>
<xml_diff>
--- a/Group_47_backlog.xlsx
+++ b/Group_47_backlog.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Desktop/SoftwareEngineeringG47/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\air\java\ruangonglab\SoftwareEngineeringG47-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C310A9F-3303-A44A-88C8-0A0B73FB4180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F812C94-F80A-45FA-AB24-5E382DBD8F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3756" yWindow="828" windowWidth="21420" windowHeight="10932" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="98">
   <si>
     <t>Story ID</t>
   </si>
@@ -52,259 +52,286 @@
     <t>1.1</t>
   </si>
   <si>
+    <t>As an administrator, I want to have a page to look at all students' information so that I can make further adjustments to one user's information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">very high  </t>
+  </si>
+  <si>
+    <t>There is a page that shows all the current students</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023.3.18  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2023.3.31</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>As an adminstrator, I want to have a page to look at all courses' information so that I can make further adjustments to courses</t>
+  </si>
+  <si>
+    <t>There is a page that shows all the current courses</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user, I want to make sure that my information is private and that I am the only person who can view my results. So I want a priavte account and the account is availble for me at anytime </t>
+  </si>
+  <si>
+    <t>Registered users can directly log in to the main interface if supply correct ID and PIN</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>As a student, I want to know how many courses I have attended exactly. So the basic module information should be listed</t>
+  </si>
+  <si>
+    <t>There should have a page link in users' personal interface, when users enter that page, they can see all the courses they are studying or have studied</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>As a user, I want to change the password and other personal information of my account to improve the security of my account</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>There is a user profile interface that allows users to change their passwords or other personal information</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>As a student, I hope not only to know how many courses I have studied, but also to intuitively know the score information of each course</t>
+  </si>
+  <si>
+    <t>When users click the grade module, they can see the grade of the course they have completed</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>As an administrator, I want to be able to add or delete or change user baisc information</t>
+  </si>
+  <si>
+    <t>Administrators can add or remove a course in course management page.</t>
+  </si>
+  <si>
+    <t>2023.4.3</t>
+  </si>
+  <si>
+    <t>2023.4.14</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As an administrator, I want to be able to add or remove a course </t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>As administrators and users, we want to be able to search quickly to find the results we want</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>Some interfaces have a search box that displays specific results when you type in a keyword</t>
+  </si>
+  <si>
+    <t>2023.4.17</t>
+  </si>
+  <si>
+    <t>2023.4.28</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>As a student, I want to be able to arrange the grades of the course in order from largest to smallest</t>
+  </si>
+  <si>
+    <t>There is a menu of options to arrange information such as grades in descending order</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>As a student, I want to be able to see the weekly curriculum schedule</t>
+  </si>
+  <si>
+    <t>There is an area in the user interface for students to see weekly curriculum schedule</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>As a student, I want to be able to see my GPA for my current completed courses</t>
+  </si>
+  <si>
+    <t>very high</t>
+  </si>
+  <si>
+    <t>Students can export their GPA on the student module grades page</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>As a user, I want my password to be invisible when I log in</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>The password is masked when the user logs in</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>As a user, I hope to have a feedback function to solve some errors in time and make the software better</t>
+  </si>
+  <si>
+    <t>There are areas for user feedback to be submitted</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>As a student, I want to see my experience of winning awards in competitions or exams at school, so I hope to have a page listing some events and awards I have participated in</t>
+  </si>
+  <si>
+    <t>There is a page to record students' personal achievements in school</t>
+  </si>
+  <si>
+    <t>2023.5.1</t>
+  </si>
+  <si>
+    <t>2023.5.12</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>As a teacher, I hope that in addition to the required courses, students themselves can have the opportunity to choose some public courses that they want to learn</t>
+  </si>
+  <si>
+    <t>In the student interface, there is a page of public courses, where students can choose some public courses to add to their module list</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t>As a student, I want to be able to log in to my personal email address to check and send messages</t>
+  </si>
+  <si>
+    <t>There is a link to access to students' email</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>As a student, I want to be able to jump directly to Google Academic webside to facilitate my search for some literature</t>
+  </si>
+  <si>
+    <t>very low</t>
+  </si>
+  <si>
+    <t>There is a link to access to literature searching website</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>As a developer, I want to beautify the software pages to give users a better user experience</t>
+  </si>
+  <si>
+    <t>The look and feel of the application interface is improved</t>
+  </si>
+  <si>
+    <t>Keyword searching</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Check for email</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Search for literature</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beautify the application interface</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>Students management</t>
-  </si>
-  <si>
-    <t>As an administrator, I want to have a page to look at all students' information so that I can make further adjustments to one user's information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">very high  </t>
-  </si>
-  <si>
-    <t>There is a page that shows all the current students</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023.3.18  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2023.3.31</t>
-  </si>
-  <si>
-    <t>1.2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Courses management</t>
-  </si>
-  <si>
-    <t>As an adminstrator, I want to have a page to look at all courses' information so that I can make further adjustments to courses</t>
-  </si>
-  <si>
-    <t>There is a page that shows all the current courses</t>
-  </si>
-  <si>
-    <t>1.3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>User login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want to make sure that my information is private and that I am the only person who can view my results. So I want a priavte account and the account is availble for me at anytime </t>
-  </si>
-  <si>
-    <t>Registered users can directly log in to the main interface if supply correct ID and PIN</t>
-  </si>
-  <si>
-    <t>1.4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>List  the module I learned</t>
-  </si>
-  <si>
-    <t>As a student, I want to know how many courses I have attended exactly. So the basic module information should be listed</t>
-  </si>
-  <si>
-    <t>There should have a page link in users' personal interface, when users enter that page, they can see all the courses they are studying or have studied</t>
-  </si>
-  <si>
-    <t>2.1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Change my personal information</t>
-  </si>
-  <si>
-    <t>As a user, I want to change the password and other personal information of my account to improve the security of my account</t>
-  </si>
-  <si>
-    <t>medium</t>
-  </si>
-  <si>
-    <t>There is a user profile interface that allows users to change their passwords or other personal information</t>
-  </si>
-  <si>
-    <t>2.2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">List student's module grades </t>
-  </si>
-  <si>
-    <t>As a student, I hope not only to know how many courses I have studied, but also to intuitively know the score information of each course</t>
-  </si>
-  <si>
-    <t>When users click the grade module, they can see the grade of the course they have completed</t>
-  </si>
-  <si>
-    <t>2.3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Add  new or delete users</t>
-  </si>
-  <si>
-    <t>As an administrator, I want to be able to add or delete or change user baisc information</t>
-  </si>
-  <si>
-    <t>Administrators can add or remove a course in course management page.</t>
-  </si>
-  <si>
-    <t>2023.4.3</t>
-  </si>
-  <si>
-    <t>2023.4.14</t>
-  </si>
-  <si>
-    <t>2.4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">Add  new or delete courses </t>
-  </si>
-  <si>
-    <t xml:space="preserve">As an administrator, I want to be able to add or remove a course </t>
-  </si>
-  <si>
-    <t>3.1</t>
-  </si>
-  <si>
-    <t>Keyword searching</t>
-  </si>
-  <si>
-    <t>As administrators and users, we want to be able to search quickly to find the results we want</t>
-  </si>
-  <si>
-    <t>high</t>
-  </si>
-  <si>
-    <t>Some interfaces have a search box that displays specific results when you type in a keyword</t>
-  </si>
-  <si>
-    <t>2023.4.17</t>
-  </si>
-  <si>
-    <t>2023.4.28</t>
-  </si>
-  <si>
-    <t>3.2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Change the arrangement of grades</t>
-  </si>
-  <si>
-    <t>As a student, I want to be able to arrange the grades of the course in order from largest to smallest</t>
-  </si>
-  <si>
-    <t>There is a menu of options to arrange information such as grades in descending order</t>
-  </si>
-  <si>
-    <t>3.3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Curriculum schedule</t>
-  </si>
-  <si>
-    <t>There is an area in the user interface for students to see weekly curriculum schedule</t>
-  </si>
-  <si>
-    <t>3.4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Export students' GPA</t>
-  </si>
-  <si>
-    <t>As a student, I want to be able to see my GPA for my current completed courses</t>
-  </si>
-  <si>
-    <t>very high</t>
-  </si>
-  <si>
-    <t>Students can export their GPA on the student module grades page</t>
-  </si>
-  <si>
-    <t>3.5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">Mask password </t>
-  </si>
-  <si>
-    <t>As a user, I want my password to be invisible when I log in</t>
-  </si>
-  <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>The password is masked when the user logs in</t>
-  </si>
-  <si>
-    <t>3.6</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Feedback</t>
-  </si>
-  <si>
-    <t>As a user, I hope to have a feedback function to solve some errors in time and make the software better</t>
-  </si>
-  <si>
-    <t>There are areas for user feedback to be submitted</t>
-  </si>
-  <si>
-    <t>4.1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Record personal achievement</t>
-  </si>
-  <si>
-    <t>As a student, I want to see my experience of winning awards in competitions or exams at school, so I hope to have a page listing some events and awards I have participated in</t>
-  </si>
-  <si>
-    <t>There is a page to record students' personal achievements in school</t>
-  </si>
-  <si>
-    <t>2023.5.1</t>
-  </si>
-  <si>
-    <t>2023.5.12</t>
-  </si>
-  <si>
-    <t>Check for email</t>
-  </si>
-  <si>
-    <t>As a student, I want to be able to log in to my personal email address to check and send messages</t>
-  </si>
-  <si>
-    <t>There is a link to access to students' email</t>
-  </si>
-  <si>
-    <t>Search for literature</t>
-  </si>
-  <si>
-    <t>As a student, I want to be able to jump directly to Google Academic webside to facilitate my search for some literature</t>
-  </si>
-  <si>
-    <t>very low</t>
-  </si>
-  <si>
-    <t>There is a link to access to literature searching website</t>
-  </si>
-  <si>
-    <t>Beautify the application interface</t>
-  </si>
-  <si>
-    <t>As a developer, I want to beautify the software pages to give users a better user experience</t>
-  </si>
-  <si>
-    <t>The look and feel of the application interface is improved</t>
-  </si>
-  <si>
-    <t>As a student, I want to be able to see the weekly curriculum schedule</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.3</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Public course selection </t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -312,7 +339,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -330,14 +357,14 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="4"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="等线"/>
-      <family val="4"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -704,26 +731,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.1640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="26.1640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" customWidth="1"/>
-    <col min="6" max="6" width="30.5" style="5" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="43.1796875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="30.6328125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="23.1796875" customWidth="1"/>
+    <col min="5" max="5" width="25.6328125" customWidth="1"/>
+    <col min="6" max="6" width="30.453125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="14.36328125" customWidth="1"/>
     <col min="8" max="8" width="38" customWidth="1"/>
-    <col min="9" max="9" width="34.33203125" customWidth="1"/>
+    <col min="9" max="9" width="34.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="17">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -752,583 +779,609 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="75.25" customHeight="1">
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="75.3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
       </c>
       <c r="F2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="115.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="116" customHeight="1">
-      <c r="A3" s="14" t="s">
+      <c r="B3" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>18</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" ht="116" customHeight="1">
+    </row>
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="115.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="70" customHeight="1">
+    </row>
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="3">
         <v>1</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" ht="126" customHeight="1">
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E6" s="3">
         <v>2</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" ht="126" customHeight="1">
+    </row>
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" s="3">
         <v>2</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" ht="51">
+    </row>
+    <row r="8" spans="1:9" s="3" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="3">
         <v>2</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="3" customFormat="1" ht="51">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="3" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" s="3">
         <v>2</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="3" customFormat="1" ht="68">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="3" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E10" s="3">
         <v>3</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="3" customFormat="1" ht="68">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="3" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E11" s="3">
         <v>3</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="3" customFormat="1" ht="51">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="3" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E12" s="3">
         <v>3</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="H12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="3" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="3" customFormat="1" ht="51">
-      <c r="A13" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="E13" s="3">
         <v>3</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="3" customFormat="1" ht="34">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="3" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E14" s="3">
         <v>3</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="3" customFormat="1" ht="68">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="3" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E15" s="3">
         <v>3</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="3" customFormat="1" ht="102">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="3" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E16" s="3">
         <v>4</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="3" customFormat="1" ht="68">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="3" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="E17" s="3">
         <v>4</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="3" customFormat="1" ht="68">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="3" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="E18" s="3">
         <v>4</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="3" customFormat="1" ht="68">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="3" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="E19" s="3">
         <v>4</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="H19" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="3" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="3">
+        <v>4</v>
+      </c>
+      <c r="F20" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="I19" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" s="3" customFormat="1">
-      <c r="A20" s="14"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="1:9" s="3" customFormat="1">
+      <c r="H20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="12"/>
       <c r="C21" s="13"/>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="1:9" s="3" customFormat="1">
+    <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="12"/>
       <c r="C22" s="13"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:9" s="3" customFormat="1">
+    <row r="23" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="12"/>
       <c r="C23" s="13"/>
       <c r="F23" s="12"/>
     </row>
-    <row r="24" spans="1:9" s="3" customFormat="1">
+    <row r="24" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="12"/>
       <c r="C24" s="13"/>
       <c r="F24" s="12"/>
     </row>
-    <row r="25" spans="1:9" s="3" customFormat="1">
+    <row r="25" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="12"/>
       <c r="C25" s="13"/>
       <c r="F25" s="12"/>
     </row>
-    <row r="26" spans="1:9" s="3" customFormat="1">
+    <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="12"/>
       <c r="C26" s="13"/>
       <c r="F26" s="12"/>
     </row>
-    <row r="27" spans="1:9" s="3" customFormat="1">
+    <row r="27" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="12"/>
       <c r="C27" s="13"/>
       <c r="F27" s="12"/>
     </row>
-    <row r="28" spans="1:9" s="3" customFormat="1">
+    <row r="28" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="12"/>
       <c r="C28" s="13"/>
       <c r="F28" s="12"/>
     </row>
-    <row r="29" spans="1:9" s="3" customFormat="1">
+    <row r="29" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="12"/>
       <c r="C29" s="13"/>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="1:9" s="3" customFormat="1">
+    <row r="30" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
       <c r="B30" s="12"/>
       <c r="C30" s="13"/>
       <c r="F30" s="12"/>
     </row>
-    <row r="31" spans="1:9" s="3" customFormat="1">
+    <row r="31" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="14"/>
       <c r="B31" s="12"/>
       <c r="C31" s="13"/>
       <c r="F31" s="12"/>
     </row>
-    <row r="32" spans="1:9" s="3" customFormat="1">
+    <row r="32" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="14"/>
       <c r="B32" s="12"/>
       <c r="C32" s="13"/>
       <c r="F32" s="12"/>
     </row>
-    <row r="33" spans="1:6" s="3" customFormat="1">
+    <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="14"/>
       <c r="B33" s="12"/>
       <c r="C33" s="13"/>
       <c r="F33" s="12"/>
     </row>
-    <row r="34" spans="1:6" s="3" customFormat="1">
+    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="14"/>
       <c r="B34" s="12"/>
       <c r="C34" s="13"/>
       <c r="F34" s="12"/>
     </row>
-    <row r="35" spans="1:6" s="3" customFormat="1">
+    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="14"/>
       <c r="B35" s="12"/>
       <c r="C35" s="13"/>
       <c r="F35" s="12"/>
     </row>
-    <row r="36" spans="1:6" s="3" customFormat="1">
+    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="14"/>
       <c r="B36" s="12"/>
       <c r="C36" s="13"/>
       <c r="F36" s="12"/>
+    </row>
+    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="14"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="13"/>
+      <c r="F37" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
almost final modify supplement some entities javadoc.
</commit_message>
<xml_diff>
--- a/Group_47_backlog.xlsx
+++ b/Group_47_backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\air\java\ruangonglab\SoftwareEngineeringG47-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Desktop/SoftwareEngineeringG47/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F812C94-F80A-45FA-AB24-5E382DBD8F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF615CA1-E6E5-E24E-A1F9-893D56ADC4E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3756" yWindow="828" windowWidth="21420" windowHeight="10932" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="94">
   <si>
     <t>Story ID</t>
   </si>
@@ -220,15 +220,6 @@
     <t>2023.5.12</t>
   </si>
   <si>
-    <t>4.2</t>
-  </si>
-  <si>
-    <t>As a teacher, I hope that in addition to the required courses, students themselves can have the opportunity to choose some public courses that they want to learn</t>
-  </si>
-  <si>
-    <t>In the student interface, there is a page of public courses, where students can choose some public courses to add to their module list</t>
-  </si>
-  <si>
     <t>4.3</t>
   </si>
   <si>
@@ -328,10 +319,6 @@
   </si>
   <si>
     <t>Record personal achievement</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Public course selection </t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -339,7 +326,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -731,26 +718,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="43.1796875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="30.6328125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="26.1796875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="23.1796875" customWidth="1"/>
-    <col min="5" max="5" width="25.6328125" customWidth="1"/>
-    <col min="6" max="6" width="30.453125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="14.36328125" customWidth="1"/>
+    <col min="1" max="1" width="43.1640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="30.5" style="5" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
     <col min="8" max="8" width="38" customWidth="1"/>
-    <col min="9" max="9" width="34.36328125" customWidth="1"/>
+    <col min="9" max="9" width="34.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="17">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -779,12 +766,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="75.3" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="75.25" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>10</v>
@@ -805,12 +792,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="115.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="116" customHeight="1">
       <c r="A3" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>16</v>
@@ -832,12 +819,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" ht="115.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="116" customHeight="1">
       <c r="A4" s="14" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>19</v>
@@ -859,12 +846,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="70" customHeight="1">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>22</v>
@@ -886,12 +873,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="126" customHeight="1">
       <c r="A6" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>25</v>
@@ -913,12 +900,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="126" customHeight="1">
       <c r="A7" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>29</v>
@@ -940,12 +927,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="3" customFormat="1" ht="51">
       <c r="A8" s="14" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>32</v>
@@ -967,12 +954,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="3" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="3" customFormat="1" ht="51">
       <c r="A9" s="14" t="s">
         <v>36</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>37</v>
@@ -994,12 +981,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="3" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" s="3" customFormat="1" ht="68">
       <c r="A10" s="14" t="s">
         <v>38</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>39</v>
@@ -1021,12 +1008,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="3" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" s="3" customFormat="1" ht="68">
       <c r="A11" s="14" t="s">
         <v>44</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>45</v>
@@ -1047,12 +1034,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="3" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="3" customFormat="1" ht="51">
       <c r="A12" s="14" t="s">
         <v>47</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>48</v>
@@ -1073,12 +1060,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="3" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" s="3" customFormat="1" ht="51">
       <c r="A13" s="14" t="s">
         <v>50</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>51</v>
@@ -1099,12 +1086,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="3" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" s="3" customFormat="1" ht="34">
       <c r="A14" s="14" t="s">
         <v>54</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>55</v>
@@ -1125,12 +1112,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="3" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" s="3" customFormat="1" ht="68">
       <c r="A15" s="14" t="s">
         <v>58</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>59</v>
@@ -1151,12 +1138,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="3" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" s="3" customFormat="1" ht="102">
       <c r="A16" s="14" t="s">
         <v>61</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>62</v>
@@ -1177,18 +1164,18 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="3" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" s="3" customFormat="1" ht="68">
       <c r="A17" s="14" t="s">
         <v>66</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>67</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="E17" s="3">
         <v>4</v>
@@ -1203,24 +1190,24 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="3" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" s="3" customFormat="1" ht="68">
       <c r="A18" s="14" t="s">
         <v>69</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>70</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="E18" s="3">
         <v>4</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>64</v>
@@ -1229,18 +1216,18 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="3" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" s="3" customFormat="1" ht="68">
       <c r="A19" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="E19" s="3">
         <v>4</v>
@@ -1255,133 +1242,107 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="3" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="3">
-        <v>4</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" s="3" customFormat="1">
+      <c r="A20" s="14"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:9" s="3" customFormat="1">
       <c r="A21" s="14"/>
       <c r="B21" s="12"/>
       <c r="C21" s="13"/>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" s="3" customFormat="1">
       <c r="A22" s="14"/>
       <c r="B22" s="12"/>
       <c r="C22" s="13"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" s="3" customFormat="1">
       <c r="A23" s="14"/>
       <c r="B23" s="12"/>
       <c r="C23" s="13"/>
       <c r="F23" s="12"/>
     </row>
-    <row r="24" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" s="3" customFormat="1">
       <c r="A24" s="14"/>
       <c r="B24" s="12"/>
       <c r="C24" s="13"/>
       <c r="F24" s="12"/>
     </row>
-    <row r="25" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" s="3" customFormat="1">
       <c r="A25" s="14"/>
       <c r="B25" s="12"/>
       <c r="C25" s="13"/>
       <c r="F25" s="12"/>
     </row>
-    <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" s="3" customFormat="1">
       <c r="A26" s="14"/>
       <c r="B26" s="12"/>
       <c r="C26" s="13"/>
       <c r="F26" s="12"/>
     </row>
-    <row r="27" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" s="3" customFormat="1">
       <c r="A27" s="14"/>
       <c r="B27" s="12"/>
       <c r="C27" s="13"/>
       <c r="F27" s="12"/>
     </row>
-    <row r="28" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" s="3" customFormat="1">
       <c r="A28" s="14"/>
       <c r="B28" s="12"/>
       <c r="C28" s="13"/>
       <c r="F28" s="12"/>
     </row>
-    <row r="29" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" s="3" customFormat="1">
       <c r="A29" s="14"/>
       <c r="B29" s="12"/>
       <c r="C29" s="13"/>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" s="3" customFormat="1">
       <c r="A30" s="14"/>
       <c r="B30" s="12"/>
       <c r="C30" s="13"/>
       <c r="F30" s="12"/>
     </row>
-    <row r="31" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" s="3" customFormat="1">
       <c r="A31" s="14"/>
       <c r="B31" s="12"/>
       <c r="C31" s="13"/>
       <c r="F31" s="12"/>
     </row>
-    <row r="32" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" s="3" customFormat="1">
       <c r="A32" s="14"/>
       <c r="B32" s="12"/>
       <c r="C32" s="13"/>
       <c r="F32" s="12"/>
     </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" s="3" customFormat="1">
       <c r="A33" s="14"/>
       <c r="B33" s="12"/>
       <c r="C33" s="13"/>
       <c r="F33" s="12"/>
     </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" s="3" customFormat="1">
       <c r="A34" s="14"/>
       <c r="B34" s="12"/>
       <c r="C34" s="13"/>
       <c r="F34" s="12"/>
     </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" s="3" customFormat="1">
       <c r="A35" s="14"/>
       <c r="B35" s="12"/>
       <c r="C35" s="13"/>
       <c r="F35" s="12"/>
     </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" s="3" customFormat="1">
       <c r="A36" s="14"/>
       <c r="B36" s="12"/>
       <c r="C36" s="13"/>
       <c r="F36" s="12"/>
-    </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="14"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="13"/>
-      <c r="F37" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>